<commit_message>
new CWE entries added
</commit_message>
<xml_diff>
--- a/CWE-List/CWE-List.xlsx
+++ b/CWE-List/CWE-List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezudilin\PT.Doc\CWE-List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\ezudilin\PT.Doc\CWE-List\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B539ACEA-921F-47CC-A468-D4C794538DD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3123" uniqueCount="3119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3397" uniqueCount="3392">
   <si>
     <t>CWE-1</t>
   </si>
@@ -9381,12 +9382,831 @@
   </si>
   <si>
     <t>DEPRECATED: Information Exposure Through Cleanup Log Files</t>
+  </si>
+  <si>
+    <t>Quality Weaknesses with Indirect Security Impacts</t>
+  </si>
+  <si>
+    <t>Use of Redundant Code</t>
+  </si>
+  <si>
+    <t>Static Member Data Element outside of a Singleton Class Element</t>
+  </si>
+  <si>
+    <t>Data Element Aggregating an Excessively Large Number of Non-Primitive Elements</t>
+  </si>
+  <si>
+    <t>Architecture with Number of Horizontal Layers Outside of Expected Range</t>
+  </si>
+  <si>
+    <t>Parent Class with a Virtual Destructor and a Child Class without a Virtual Destructor</t>
+  </si>
+  <si>
+    <t>Creation of Immutable Text Using String Concatenation</t>
+  </si>
+  <si>
+    <t>Modules with Circular Dependencies</t>
+  </si>
+  <si>
+    <t>Invokable Control Element with Large Number of Outward Calls</t>
+  </si>
+  <si>
+    <t>Excessive Data Query Operations in a Large Data Table</t>
+  </si>
+  <si>
+    <t>Excessive Platform Resource Consumption within a Loop</t>
+  </si>
+  <si>
+    <t>Initialization with Hard-Coded Network Resource Configuration Data</t>
+  </si>
+  <si>
+    <t>Excessive Use of Hard-Coded Literals in Initialization</t>
+  </si>
+  <si>
+    <t>Missing Documentation for Design</t>
+  </si>
+  <si>
+    <t>Invocation of a Control Element at an Unnecessarily Deep Horizontal Layer</t>
+  </si>
+  <si>
+    <t>Multiple Inheritance from Concrete Classes</t>
+  </si>
+  <si>
+    <t>Invokable Control Element with Variadic Parameters</t>
+  </si>
+  <si>
+    <t>Data Access Operations Outside of Expected Data Manager Component</t>
+  </si>
+  <si>
+    <t>Invokable Control Element in Multi-Thread Context with non-Final Static Storable or Member Element</t>
+  </si>
+  <si>
+    <t>Incomplete Documentation</t>
+  </si>
+  <si>
+    <t>Excessive Number of Inefficient Server-Side Data Accesses</t>
+  </si>
+  <si>
+    <t>Parent Class with References to Child Class</t>
+  </si>
+  <si>
+    <t>Creation of Class Instance within a Static Code Block</t>
+  </si>
+  <si>
+    <t>Invokable Control Element with Signature Containing an Excessive Number of Parameters</t>
+  </si>
+  <si>
+    <t>Runtime Resource Management Control Element in a Component Built to Run on Application Servers</t>
+  </si>
+  <si>
+    <t>Missing Serialization Control Element</t>
+  </si>
+  <si>
+    <t>Excessive Execution of Sequential Searches of Data Resource</t>
+  </si>
+  <si>
+    <t>Inconsistency Between Implementation and Documented Design</t>
+  </si>
+  <si>
+    <t>Empty Exception Block</t>
+  </si>
+  <si>
+    <t>Serializable Data Element Containing non-Serializable Item Elements</t>
+  </si>
+  <si>
+    <t>Empty Code Block</t>
+  </si>
+  <si>
+    <t>Data Resource Access without Use of Connection Pooling</t>
+  </si>
+  <si>
+    <t>Non-SQL Invokable Control Element with Excessive Number of Data Resource Accesses</t>
+  </si>
+  <si>
+    <t>Class with Excessively Deep Inheritance</t>
+  </si>
+  <si>
+    <t>Unconditional Control Flow Transfer outside of Switch Block</t>
+  </si>
+  <si>
+    <t>Insufficient Adherence to Expected Conventions</t>
+  </si>
+  <si>
+    <t>Floating Point Comparison with Incorrect Operator</t>
+  </si>
+  <si>
+    <t>Inappropriate Source Code Style or Formatting</t>
+  </si>
+  <si>
+    <t>Parent Class without Virtual Destructor Method</t>
+  </si>
+  <si>
+    <t>Source Code File with Excessive Number of Lines of Code</t>
+  </si>
+  <si>
+    <t>Class Instance Self Destruction Control Element</t>
+  </si>
+  <si>
+    <t>Data Access from Outside Expected Data Manager Component</t>
+  </si>
+  <si>
+    <t>Invokable Control Element with Excessive File or Data Access Operations</t>
+  </si>
+  <si>
+    <t>Invokable Control Element with Excessive Volume of Commented-out Code</t>
+  </si>
+  <si>
+    <t>Class with Excessive Number of Child Classes</t>
+  </si>
+  <si>
+    <t>Class with Virtual Method without a Virtual Destructor</t>
+  </si>
+  <si>
+    <t>Synchronous Access of Remote Resource without Timeout</t>
+  </si>
+  <si>
+    <t>Large Data Table with Excessive Number of Indices</t>
+  </si>
+  <si>
+    <t>Method Containing Access of a Member Element from Another Class</t>
+  </si>
+  <si>
+    <t>Use of Object without Invoking Destructor Method</t>
+  </si>
+  <si>
+    <t>Use of Same Invokable Control Element in Multiple Architectural Layers</t>
+  </si>
+  <si>
+    <t>Excessively Complex Data Representation</t>
+  </si>
+  <si>
+    <t>Excessive Index Range Scan for a Data Resource</t>
+  </si>
+  <si>
+    <t>Loop Condition Value Update within the Loop</t>
+  </si>
+  <si>
+    <t>Singleton Class Instance Creation without Proper Locking or Synchronization</t>
+  </si>
+  <si>
+    <t>Persistent Storable Data Element without Associated Comparison Control Element</t>
+  </si>
+  <si>
+    <t>Data Element containing Pointer Item without Proper Copy Control Element</t>
+  </si>
+  <si>
+    <t>Inconsistent Naming Conventions for Identifiers</t>
+  </si>
+  <si>
+    <t>Insufficient Isolation of System-Dependent Functions</t>
+  </si>
+  <si>
+    <t>Reliance on Runtime Component in Generated Code</t>
+  </si>
+  <si>
+    <t>Reliance on Machine-Dependent Data Representation</t>
+  </si>
+  <si>
+    <t>Use of Platform-Dependent Third Party Components</t>
+  </si>
+  <si>
+    <t>Use of Unmaintained Third Party Components</t>
+  </si>
+  <si>
+    <t>Insufficient Encapsulation of Machine-Dependent Functionality</t>
+  </si>
+  <si>
+    <t>Insufficient Use of Symbolic Constants</t>
+  </si>
+  <si>
+    <t>Insufficient Isolation of Symbolic Constant Definitions</t>
+  </si>
+  <si>
+    <t>Excessive Reliance on Global Variables</t>
+  </si>
+  <si>
+    <t>Use of Same Variable for Multiple Purposes</t>
+  </si>
+  <si>
+    <t>Incomplete Design Documentation</t>
+  </si>
+  <si>
+    <t>Incomplete I/O Documentation</t>
+  </si>
+  <si>
+    <t>Incomplete Documentation of Program Execution</t>
+  </si>
+  <si>
+    <t>Inappropriate Comment Style</t>
+  </si>
+  <si>
+    <t>Inappropriate Whitespace Style</t>
+  </si>
+  <si>
+    <t>Source Code Element without Standard Prologue</t>
+  </si>
+  <si>
+    <t>Inaccurate Comments</t>
+  </si>
+  <si>
+    <t>Callable with Insufficient Behavioral Summary</t>
+  </si>
+  <si>
+    <t>Insufficient Documentation of Error Handling Techniques</t>
+  </si>
+  <si>
+    <t>Excessive Use of Unconditional Branching</t>
+  </si>
+  <si>
+    <t>Excessive Code Complexity</t>
+  </si>
+  <si>
+    <t>Excessive McCabe Cyclomatic Complexity</t>
+  </si>
+  <si>
+    <t>Excessive Halstead Complexity</t>
+  </si>
+  <si>
+    <t>Excessive Use of Self-Modifying Code</t>
+  </si>
+  <si>
+    <t>Excessively Deep Nesting</t>
+  </si>
+  <si>
+    <t>Excessive Attack Surface</t>
+  </si>
+  <si>
+    <t>Declaration of Variable with Unnecessarily Wide Scope</t>
+  </si>
+  <si>
+    <t>Compilation with Insufficient Warnings or Errors</t>
+  </si>
+  <si>
+    <t>CISQ Quality Measures (2016)</t>
+  </si>
+  <si>
+    <t>CISQ Quality Measures - Reliability</t>
+  </si>
+  <si>
+    <t>CISQ Quality Measures - Maintainability</t>
+  </si>
+  <si>
+    <t>CISQ Quality Measures - Security</t>
+  </si>
+  <si>
+    <t>CISQ Quality Measures - Performance</t>
+  </si>
+  <si>
+    <t>Weaknesses Addressed by the SEI CERT Oracle Coding Standard for Java</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 00. Input Validation and Data Sanitization (IDS)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 01. Declarations and Initialization (DCL)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 02. Expressions (EXP)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 03. Numeric Types and Operations (NUM)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 04. Characters and Strings (STR)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 05. Object Orientation (OBJ)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 06. Methods (MET)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 07. Exceptional Behavior (ERR)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 08. Visibility and Atomicity (VNA)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 09. Locking (LCK)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 10. Thread APIs (THI)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 11. Thread Pools (TPS)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 12. Thread-Safety Miscellaneous (TSM)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 13. Input Output (FIO)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 14. Serialization (SER)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 15. Platform Security (SEC)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 16. Runtime Environment (ENV)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 17. Java Native Interface (JNI)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 49. Miscellaneous (MSC)</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 50. Android (DRD)</t>
+  </si>
+  <si>
+    <t>Weaknesses Addressed by the SEI CERT C Coding Standard</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 01. Preprocessor (PRE)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 02. Declarations and Initialization (DCL)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 03. Expressions (EXP)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 04. Integers (INT)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 05. Floating Point (FLP)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 06. Arrays (ARR)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 07. Characters and Strings (STR)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 08. Memory Management (MEM)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 09. Input Output (FIO)</t>
+  </si>
+  <si>
+    <t>Irrelevant Code</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 10. Environment (ENV)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 11. Signals (SIG)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 12. Error Handling (ERR)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 13. Application Programming Interfaces (API)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 14. Concurrency (CON)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 48. Miscellaneous (MSC)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 50. POSIX (POS)</t>
+  </si>
+  <si>
+    <t>SEI CERT C Coding Standard - Guidelines 51. Microsoft Windows (WIN)</t>
+  </si>
+  <si>
+    <t>Improper Use of Validation Framework</t>
+  </si>
+  <si>
+    <t>ASP.NET Misconfiguration: Improper Model Validation</t>
+  </si>
+  <si>
+    <t>SEI CERT Oracle Secure Coding Standard for Java - Guidelines 18. Concurrency (CON)</t>
+  </si>
+  <si>
+    <t>Inefficient CPU Computation</t>
+  </si>
+  <si>
+    <t>Use of Prohibited Code</t>
+  </si>
+  <si>
+    <t>CWE-1040</t>
+  </si>
+  <si>
+    <t>CWE-1041</t>
+  </si>
+  <si>
+    <t>CWE-1042</t>
+  </si>
+  <si>
+    <t>CWE-1043</t>
+  </si>
+  <si>
+    <t>CWE-1044</t>
+  </si>
+  <si>
+    <t>CWE-1045</t>
+  </si>
+  <si>
+    <t>CWE-1046</t>
+  </si>
+  <si>
+    <t>CWE-1047</t>
+  </si>
+  <si>
+    <t>CWE-1048</t>
+  </si>
+  <si>
+    <t>CWE-1049</t>
+  </si>
+  <si>
+    <t>CWE-1050</t>
+  </si>
+  <si>
+    <t>CWE-1051</t>
+  </si>
+  <si>
+    <t>CWE-1052</t>
+  </si>
+  <si>
+    <t>CWE-1053</t>
+  </si>
+  <si>
+    <t>CWE-1054</t>
+  </si>
+  <si>
+    <t>CWE-1055</t>
+  </si>
+  <si>
+    <t>CWE-1056</t>
+  </si>
+  <si>
+    <t>CWE-1057</t>
+  </si>
+  <si>
+    <t>CWE-1058</t>
+  </si>
+  <si>
+    <t>CWE-1059</t>
+  </si>
+  <si>
+    <t>CWE-1060</t>
+  </si>
+  <si>
+    <t>CWE-1061</t>
+  </si>
+  <si>
+    <t>CWE-1062</t>
+  </si>
+  <si>
+    <t>CWE-1063</t>
+  </si>
+  <si>
+    <t>CWE-1064</t>
+  </si>
+  <si>
+    <t>CWE-1065</t>
+  </si>
+  <si>
+    <t>CWE-1066</t>
+  </si>
+  <si>
+    <t>CWE-1067</t>
+  </si>
+  <si>
+    <t>CWE-1068</t>
+  </si>
+  <si>
+    <t>CWE-1069</t>
+  </si>
+  <si>
+    <t>CWE-1070</t>
+  </si>
+  <si>
+    <t>CWE-1071</t>
+  </si>
+  <si>
+    <t>CWE-1072</t>
+  </si>
+  <si>
+    <t>CWE-1073</t>
+  </si>
+  <si>
+    <t>CWE-1074</t>
+  </si>
+  <si>
+    <t>CWE-1075</t>
+  </si>
+  <si>
+    <t>CWE-1076</t>
+  </si>
+  <si>
+    <t>CWE-1077</t>
+  </si>
+  <si>
+    <t>CWE-1078</t>
+  </si>
+  <si>
+    <t>CWE-1079</t>
+  </si>
+  <si>
+    <t>CWE-1080</t>
+  </si>
+  <si>
+    <t>CWE-1082</t>
+  </si>
+  <si>
+    <t>CWE-1083</t>
+  </si>
+  <si>
+    <t>CWE-1084</t>
+  </si>
+  <si>
+    <t>CWE-1085</t>
+  </si>
+  <si>
+    <t>CWE-1086</t>
+  </si>
+  <si>
+    <t>CWE-1087</t>
+  </si>
+  <si>
+    <t>CWE-1088</t>
+  </si>
+  <si>
+    <t>CWE-1089</t>
+  </si>
+  <si>
+    <t>CWE-1090</t>
+  </si>
+  <si>
+    <t>CWE-1091</t>
+  </si>
+  <si>
+    <t>CWE-1092</t>
+  </si>
+  <si>
+    <t>CWE-1093</t>
+  </si>
+  <si>
+    <t>CWE-1094</t>
+  </si>
+  <si>
+    <t>CWE-1095</t>
+  </si>
+  <si>
+    <t>CWE-1096</t>
+  </si>
+  <si>
+    <t>CWE-1097</t>
+  </si>
+  <si>
+    <t>CWE-1098</t>
+  </si>
+  <si>
+    <t>CWE-1099</t>
+  </si>
+  <si>
+    <t>CWE-1100</t>
+  </si>
+  <si>
+    <t>CWE-1101</t>
+  </si>
+  <si>
+    <t>CWE-1102</t>
+  </si>
+  <si>
+    <t>CWE-1103</t>
+  </si>
+  <si>
+    <t>CWE-1104</t>
+  </si>
+  <si>
+    <t>CWE-1105</t>
+  </si>
+  <si>
+    <t>CWE-1106</t>
+  </si>
+  <si>
+    <t>CWE-1107</t>
+  </si>
+  <si>
+    <t>CWE-1108</t>
+  </si>
+  <si>
+    <t>CWE-1109</t>
+  </si>
+  <si>
+    <t>CWE-1110</t>
+  </si>
+  <si>
+    <t>CWE-1111</t>
+  </si>
+  <si>
+    <t>CWE-1112</t>
+  </si>
+  <si>
+    <t>CWE-1113</t>
+  </si>
+  <si>
+    <t>CWE-1114</t>
+  </si>
+  <si>
+    <t>CWE-1115</t>
+  </si>
+  <si>
+    <t>CWE-1116</t>
+  </si>
+  <si>
+    <t>CWE-1117</t>
+  </si>
+  <si>
+    <t>CWE-1118</t>
+  </si>
+  <si>
+    <t>CWE-1119</t>
+  </si>
+  <si>
+    <t>CWE-1120</t>
+  </si>
+  <si>
+    <t>CWE-1121</t>
+  </si>
+  <si>
+    <t>CWE-1122</t>
+  </si>
+  <si>
+    <t>CWE-1123</t>
+  </si>
+  <si>
+    <t>CWE-1124</t>
+  </si>
+  <si>
+    <t>CWE-1125</t>
+  </si>
+  <si>
+    <t>CWE-1126</t>
+  </si>
+  <si>
+    <t>CWE-1127</t>
+  </si>
+  <si>
+    <t>CWE-1128</t>
+  </si>
+  <si>
+    <t>CWE-1129</t>
+  </si>
+  <si>
+    <t>CWE-1130</t>
+  </si>
+  <si>
+    <t>CWE-1131</t>
+  </si>
+  <si>
+    <t>CWE-1132</t>
+  </si>
+  <si>
+    <t>CWE-1133</t>
+  </si>
+  <si>
+    <t>CWE-1134</t>
+  </si>
+  <si>
+    <t>CWE-1135</t>
+  </si>
+  <si>
+    <t>CWE-1136</t>
+  </si>
+  <si>
+    <t>CWE-1137</t>
+  </si>
+  <si>
+    <t>CWE-1138</t>
+  </si>
+  <si>
+    <t>CWE-1139</t>
+  </si>
+  <si>
+    <t>CWE-1140</t>
+  </si>
+  <si>
+    <t>CWE-1141</t>
+  </si>
+  <si>
+    <t>CWE-1142</t>
+  </si>
+  <si>
+    <t>CWE-1143</t>
+  </si>
+  <si>
+    <t>CWE-1144</t>
+  </si>
+  <si>
+    <t>CWE-1145</t>
+  </si>
+  <si>
+    <t>CWE-1146</t>
+  </si>
+  <si>
+    <t>CWE-1147</t>
+  </si>
+  <si>
+    <t>CWE-1148</t>
+  </si>
+  <si>
+    <t>CWE-1149</t>
+  </si>
+  <si>
+    <t>CWE-1150</t>
+  </si>
+  <si>
+    <t>CWE-1151</t>
+  </si>
+  <si>
+    <t>CWE-1152</t>
+  </si>
+  <si>
+    <t>CWE-1153</t>
+  </si>
+  <si>
+    <t>CWE-1154</t>
+  </si>
+  <si>
+    <t>CWE-1155</t>
+  </si>
+  <si>
+    <t>CWE-1156</t>
+  </si>
+  <si>
+    <t>CWE-1157</t>
+  </si>
+  <si>
+    <t>CWE-1158</t>
+  </si>
+  <si>
+    <t>CWE-1159</t>
+  </si>
+  <si>
+    <t>CWE-1160</t>
+  </si>
+  <si>
+    <t>CWE-1161</t>
+  </si>
+  <si>
+    <t>CWE-1162</t>
+  </si>
+  <si>
+    <t>CWE-1163</t>
+  </si>
+  <si>
+    <t>CWE-1164</t>
+  </si>
+  <si>
+    <t>CWE-1165</t>
+  </si>
+  <si>
+    <t>CWE-1166</t>
+  </si>
+  <si>
+    <t>CWE-1167</t>
+  </si>
+  <si>
+    <t>CWE-1168</t>
+  </si>
+  <si>
+    <t>CWE-1169</t>
+  </si>
+  <si>
+    <t>CWE-1170</t>
+  </si>
+  <si>
+    <t>CWE-1171</t>
+  </si>
+  <si>
+    <t>CWE-1172</t>
+  </si>
+  <si>
+    <t>CWE-1173</t>
+  </si>
+  <si>
+    <t>CWE-1174</t>
+  </si>
+  <si>
+    <t>CWE-1175</t>
+  </si>
+  <si>
+    <t>CWE-1176</t>
+  </si>
+  <si>
+    <t>CWE-1177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -9559,72 +10379,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFF44CE0"/>
     </mruColors>
@@ -9641,12 +10395,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:C1041" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C1041"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:C1040" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C1040" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="ID" dataDxfId="2"/>
-    <tableColumn id="2" name="ENG" dataDxfId="1"/>
-    <tableColumn id="3" name="RUS" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ENG" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="RUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9660,7 +10414,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="A0A0A0"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -9914,18 +10668,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1041"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1022" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B543" sqref="B543"/>
+    <sheetView tabSelected="1" topLeftCell="A1024" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1041" sqref="C1041"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="84.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -21369,14 +22123,1110 @@
         <v>2879</v>
       </c>
     </row>
-    <row r="1041" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1041" s="3" t="s">
+    <row r="1041" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1041" s="1" t="s">
+        <v>3255</v>
+      </c>
+      <c r="B1041" s="1" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1042" s="1" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B1042" s="1" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1043" s="1" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B1043" s="1" t="s">
+        <v>3121</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1044" s="1" t="s">
+        <v>3258</v>
+      </c>
+      <c r="B1044" s="1" t="s">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1045" s="1" t="s">
+        <v>3259</v>
+      </c>
+      <c r="B1045" s="1" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1046" s="1" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B1046" s="1" t="s">
+        <v>3124</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1047" s="1" t="s">
+        <v>3261</v>
+      </c>
+      <c r="B1047" s="1" t="s">
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1048" s="1" t="s">
+        <v>3262</v>
+      </c>
+      <c r="B1048" s="1" t="s">
+        <v>3126</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1049" s="1" t="s">
+        <v>3263</v>
+      </c>
+      <c r="B1049" s="1" t="s">
+        <v>3127</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1050" s="1" t="s">
+        <v>3264</v>
+      </c>
+      <c r="B1050" s="1" t="s">
+        <v>3128</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1051" s="1" t="s">
+        <v>3265</v>
+      </c>
+      <c r="B1051" s="1" t="s">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1052" s="1" t="s">
+        <v>3266</v>
+      </c>
+      <c r="B1052" s="1" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1053" s="1" t="s">
+        <v>3267</v>
+      </c>
+      <c r="B1053" s="1" t="s">
+        <v>3131</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1054" s="1" t="s">
+        <v>3268</v>
+      </c>
+      <c r="B1054" s="1" t="s">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1055" s="1" t="s">
+        <v>3269</v>
+      </c>
+      <c r="B1055" s="1" t="s">
+        <v>3133</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1056" s="1" t="s">
+        <v>3270</v>
+      </c>
+      <c r="B1056" s="1" t="s">
+        <v>3134</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1057" s="1" t="s">
+        <v>3271</v>
+      </c>
+      <c r="B1057" s="1" t="s">
+        <v>3135</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1058" s="1" t="s">
+        <v>3272</v>
+      </c>
+      <c r="B1058" s="1" t="s">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1059" s="1" t="s">
+        <v>3273</v>
+      </c>
+      <c r="B1059" s="1" t="s">
+        <v>3137</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1060" s="1" t="s">
+        <v>3274</v>
+      </c>
+      <c r="B1060" s="1" t="s">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1061" s="1" t="s">
+        <v>3275</v>
+      </c>
+      <c r="B1061" s="1" t="s">
+        <v>3139</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1062" s="1" t="s">
+        <v>3276</v>
+      </c>
+      <c r="B1062" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1063" s="1" t="s">
+        <v>3277</v>
+      </c>
+      <c r="B1063" s="1" t="s">
+        <v>3140</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1064" s="1" t="s">
+        <v>3278</v>
+      </c>
+      <c r="B1064" s="1" t="s">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1065" s="1" t="s">
+        <v>3279</v>
+      </c>
+      <c r="B1065" s="1" t="s">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1066" s="1" t="s">
+        <v>3280</v>
+      </c>
+      <c r="B1066" s="1" t="s">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1067" s="1" t="s">
+        <v>3281</v>
+      </c>
+      <c r="B1067" s="1" t="s">
+        <v>3144</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1068" s="1" t="s">
+        <v>3282</v>
+      </c>
+      <c r="B1068" s="1" t="s">
+        <v>3145</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1069" s="1" t="s">
+        <v>3283</v>
+      </c>
+      <c r="B1069" s="1" t="s">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1070" s="1" t="s">
+        <v>3284</v>
+      </c>
+      <c r="B1070" s="1" t="s">
+        <v>3147</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1071" s="1" t="s">
+        <v>3285</v>
+      </c>
+      <c r="B1071" s="1" t="s">
+        <v>3148</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1072" s="1" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B1072" s="1" t="s">
+        <v>3149</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1073" s="1" t="s">
+        <v>3287</v>
+      </c>
+      <c r="B1073" s="1" t="s">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1074" s="1" t="s">
+        <v>3288</v>
+      </c>
+      <c r="B1074" s="1" t="s">
+        <v>3151</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1" t="s">
+        <v>3289</v>
+      </c>
+      <c r="B1075" s="1" t="s">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1076" s="1" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B1076" s="1" t="s">
+        <v>3153</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1077" s="1" t="s">
+        <v>3291</v>
+      </c>
+      <c r="B1077" s="1" t="s">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1078" s="1" t="s">
+        <v>3292</v>
+      </c>
+      <c r="B1078" s="1" t="s">
+        <v>3155</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1079" s="1" t="s">
+        <v>3293</v>
+      </c>
+      <c r="B1079" s="1" t="s">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1080" s="1" t="s">
+        <v>3294</v>
+      </c>
+      <c r="B1080" s="1" t="s">
+        <v>3157</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1081" s="1" t="s">
+        <v>3295</v>
+      </c>
+      <c r="B1081" s="1" t="s">
+        <v>3158</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1082" s="1" t="s">
+        <v>3296</v>
+      </c>
+      <c r="B1082" s="1" t="s">
+        <v>3159</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1083" s="1" t="s">
+        <v>3297</v>
+      </c>
+      <c r="B1083" s="1" t="s">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1084" s="1" t="s">
+        <v>3298</v>
+      </c>
+      <c r="B1084" s="1" t="s">
+        <v>3161</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1085" s="1" t="s">
+        <v>3299</v>
+      </c>
+      <c r="B1085" s="1" t="s">
+        <v>3162</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1086" s="1" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B1086" s="1" t="s">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1087" s="1" t="s">
+        <v>3301</v>
+      </c>
+      <c r="B1087" s="1" t="s">
+        <v>3164</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1088" s="1" t="s">
+        <v>3302</v>
+      </c>
+      <c r="B1088" s="1" t="s">
+        <v>3165</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1089" s="1" t="s">
+        <v>3303</v>
+      </c>
+      <c r="B1089" s="1" t="s">
+        <v>3166</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1090" s="1" t="s">
+        <v>3304</v>
+      </c>
+      <c r="B1090" s="1" t="s">
+        <v>3167</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1091" s="1" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B1091" s="1" t="s">
+        <v>3168</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1092" s="1" t="s">
+        <v>3306</v>
+      </c>
+      <c r="B1092" s="1" t="s">
+        <v>3169</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1093" s="1" t="s">
+        <v>3307</v>
+      </c>
+      <c r="B1093" s="1" t="s">
+        <v>3170</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1094" s="1" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B1094" s="1" t="s">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1095" s="1" t="s">
+        <v>3309</v>
+      </c>
+      <c r="B1095" s="1" t="s">
+        <v>3172</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1096" s="1" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B1096" s="1" t="s">
+        <v>3173</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1097" s="1" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B1097" s="1" t="s">
+        <v>3174</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1098" s="1" t="s">
+        <v>3312</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1099" s="1" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>3176</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1100" s="1" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B1100" s="1" t="s">
+        <v>3177</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1101" s="1" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B1101" s="1" t="s">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1102" s="1" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B1102" s="1" t="s">
+        <v>3179</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1103" s="1" t="s">
+        <v>3317</v>
+      </c>
+      <c r="B1103" s="1" t="s">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1104" s="1" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B1104" s="1" t="s">
+        <v>3181</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1105" s="1" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B1105" s="1" t="s">
+        <v>3182</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1106" s="1" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B1106" s="1" t="s">
+        <v>3183</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1107" s="1" t="s">
+        <v>3321</v>
+      </c>
+      <c r="B1107" s="1" t="s">
+        <v>3184</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1108" s="1" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B1108" s="1" t="s">
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1109" s="1" t="s">
+        <v>3323</v>
+      </c>
+      <c r="B1109" s="1" t="s">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1110" s="1" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B1110" s="1" t="s">
+        <v>3187</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1111" s="1" t="s">
+        <v>3325</v>
+      </c>
+      <c r="B1111" s="1" t="s">
+        <v>3188</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1112" s="1" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B1112" s="1" t="s">
+        <v>3189</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1113" s="1" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B1113" s="1" t="s">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1114" s="1" t="s">
+        <v>3328</v>
+      </c>
+      <c r="B1114" s="1" t="s">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1115" s="1" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B1115" s="1" t="s">
+        <v>3192</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1116" s="1" t="s">
+        <v>3330</v>
+      </c>
+      <c r="B1116" s="1" t="s">
+        <v>3193</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1117" s="1" t="s">
+        <v>3331</v>
+      </c>
+      <c r="B1117" s="1" t="s">
+        <v>3194</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1118" s="1" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B1118" s="1" t="s">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1119" s="1" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B1119" s="1" t="s">
+        <v>3196</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1120" s="1" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B1120" s="1" t="s">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1121" s="1" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B1121" s="1" t="s">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1122" s="1" t="s">
+        <v>3336</v>
+      </c>
+      <c r="B1122" s="1" t="s">
+        <v>3199</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1123" s="1" t="s">
+        <v>3337</v>
+      </c>
+      <c r="B1123" s="1" t="s">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1124" s="1" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B1124" s="1" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1125" s="1" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B1125" s="1" t="s">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1126" s="1" t="s">
+        <v>3340</v>
+      </c>
+      <c r="B1126" s="1" t="s">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1127" s="1" t="s">
+        <v>3341</v>
+      </c>
+      <c r="B1127" s="1" t="s">
+        <v>3204</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1128" s="1" t="s">
+        <v>3342</v>
+      </c>
+      <c r="B1128" s="1" t="s">
+        <v>3205</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1129" s="1" t="s">
+        <v>3343</v>
+      </c>
+      <c r="B1129" s="1" t="s">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1130" s="1" t="s">
+        <v>3344</v>
+      </c>
+      <c r="B1130" s="1" t="s">
+        <v>3207</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1131" s="1" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B1131" s="1" t="s">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1132" s="1" t="s">
+        <v>3346</v>
+      </c>
+      <c r="B1132" s="1" t="s">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1133" s="1" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B1133" s="1" t="s">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1134" s="1" t="s">
+        <v>3348</v>
+      </c>
+      <c r="B1134" s="1" t="s">
+        <v>3211</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1135" s="1" t="s">
+        <v>3349</v>
+      </c>
+      <c r="B1135" s="1" t="s">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1136" s="1" t="s">
+        <v>3350</v>
+      </c>
+      <c r="B1136" s="1" t="s">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1137" s="1" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B1137" s="1" t="s">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1138" s="1" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B1138" s="1" t="s">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1139" s="1" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B1139" s="1" t="s">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1140" s="1" t="s">
+        <v>3354</v>
+      </c>
+      <c r="B1140" s="1" t="s">
+        <v>3217</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1141" s="1" t="s">
+        <v>3355</v>
+      </c>
+      <c r="B1141" s="1" t="s">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1142" s="1" t="s">
+        <v>3356</v>
+      </c>
+      <c r="B1142" s="1" t="s">
+        <v>3219</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1143" s="1" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1143" s="1" t="s">
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1144" s="1" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B1144" s="1" t="s">
+        <v>3221</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1145" s="1" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B1145" s="1" t="s">
+        <v>3222</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1146" s="1" t="s">
+        <v>3360</v>
+      </c>
+      <c r="B1146" s="1" t="s">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1147" s="1" t="s">
+        <v>3361</v>
+      </c>
+      <c r="B1147" s="1" t="s">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1148" s="1" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B1148" s="1" t="s">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1149" s="1" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B1149" s="1" t="s">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1150" s="1" t="s">
+        <v>3364</v>
+      </c>
+      <c r="B1150" s="1" t="s">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1151" s="1" t="s">
+        <v>3365</v>
+      </c>
+      <c r="B1151" s="1" t="s">
+        <v>3228</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1152" s="1" t="s">
+        <v>3366</v>
+      </c>
+      <c r="B1152" s="1" t="s">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1153" s="1" t="s">
+        <v>3367</v>
+      </c>
+      <c r="B1153" s="1" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1154" s="1" t="s">
+        <v>3368</v>
+      </c>
+      <c r="B1154" s="1" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1155" s="1" t="s">
+        <v>3369</v>
+      </c>
+      <c r="B1155" s="1" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1156" s="1" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B1156" s="1" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1157" s="1" t="s">
+        <v>3371</v>
+      </c>
+      <c r="B1157" s="1" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1158" s="1" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B1158" s="1" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1159" s="1" t="s">
+        <v>3373</v>
+      </c>
+      <c r="B1159" s="1" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1160" s="1" t="s">
+        <v>3374</v>
+      </c>
+      <c r="B1160" s="1" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1161" s="1" t="s">
+        <v>3375</v>
+      </c>
+      <c r="B1161" s="1" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1162" s="1" t="s">
+        <v>3376</v>
+      </c>
+      <c r="B1162" s="1" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1163" s="1" t="s">
+        <v>3377</v>
+      </c>
+      <c r="B1163" s="1" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1164" s="1" t="s">
+        <v>3378</v>
+      </c>
+      <c r="B1164" s="1" t="s">
+        <v>3241</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1165" s="1" t="s">
+        <v>3379</v>
+      </c>
+      <c r="B1165" s="1" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1166" s="1" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B1166" s="1" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1167" s="1" t="s">
+        <v>3381</v>
+      </c>
+      <c r="B1167" s="1" t="s">
+        <v>3244</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1168" s="1" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B1168" s="1" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1169" s="1" t="s">
+        <v>3383</v>
+      </c>
+      <c r="B1169" s="1" t="s">
+        <v>3246</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1170" s="1" t="s">
+        <v>3384</v>
+      </c>
+      <c r="B1170" s="1" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1171" s="1" t="s">
+        <v>3385</v>
+      </c>
+      <c r="B1171" s="1" t="s">
+        <v>3248</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1172" s="1" t="s">
+        <v>3386</v>
+      </c>
+      <c r="B1172" s="1" t="s">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1173" s="1" t="s">
+        <v>3387</v>
+      </c>
+      <c r="B1173" s="1" t="s">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1174" s="1" t="s">
+        <v>3388</v>
+      </c>
+      <c r="B1174" s="1" t="s">
+        <v>3251</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1175" s="1" t="s">
+        <v>3389</v>
+      </c>
+      <c r="B1175" s="1" t="s">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1176" s="1" t="s">
+        <v>3390</v>
+      </c>
+      <c r="B1176" s="1" t="s">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1177" s="1" t="s">
+        <v>3391</v>
+      </c>
+      <c r="B1177" s="1" t="s">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1178" s="3" t="s">
         <v>1975</v>
       </c>
-      <c r="B1041" s="1" t="s">
+      <c r="B1178" s="1" t="s">
         <v>1976</v>
       </c>
-      <c r="C1041" s="1" t="s">
+      <c r="C1178" s="1" t="s">
         <v>2452</v>
       </c>
     </row>

</xml_diff>